<commit_message>
- arreglo para b en caso de 1 proceso
</commit_message>
<xml_diff>
--- a/Formula para calculo de B.xlsx
+++ b/Formula para calculo de B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.esquivel\Desktop\Carlos\Arqui\Tarea programada mpi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9B7ECD-F51A-4973-B9A7-B8B08D365A28}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD66CD33-A693-4E2C-B855-1D5C6271753E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{A4AA1885-9F2B-4D75-99D5-AA4B849C16D4}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{A4AA1885-9F2B-4D75-99D5-AA4B849C16D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6E11F-98EC-4B58-8955-7D676986A193}">
-  <dimension ref="B2:P37"/>
+  <dimension ref="B2:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23:P37"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2122,6 +2118,1372 @@
         <v>44</v>
       </c>
     </row>
+    <row r="42" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>5</v>
+      </c>
+      <c r="G43" s="2">
+        <v>6</v>
+      </c>
+      <c r="H43" s="2">
+        <v>7</v>
+      </c>
+      <c r="I43" s="2">
+        <v>8</v>
+      </c>
+      <c r="J43" s="2">
+        <v>9</v>
+      </c>
+      <c r="K43" s="2">
+        <v>10</v>
+      </c>
+      <c r="L43" s="2">
+        <v>11</v>
+      </c>
+      <c r="M43" s="2">
+        <v>12</v>
+      </c>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>5</v>
+      </c>
+      <c r="G44" s="4">
+        <v>6</v>
+      </c>
+      <c r="H44" s="4">
+        <v>7</v>
+      </c>
+      <c r="I44" s="4">
+        <v>8</v>
+      </c>
+      <c r="J44" s="4">
+        <v>9</v>
+      </c>
+      <c r="K44" s="4">
+        <v>10</v>
+      </c>
+      <c r="L44" s="4">
+        <v>11</v>
+      </c>
+      <c r="M44" s="4">
+        <v>12</v>
+      </c>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4">
+        <v>2</v>
+      </c>
+      <c r="D45" s="4">
+        <v>3</v>
+      </c>
+      <c r="E45" s="4">
+        <v>4</v>
+      </c>
+      <c r="F45" s="4">
+        <v>5</v>
+      </c>
+      <c r="G45" s="4">
+        <v>6</v>
+      </c>
+      <c r="H45" s="4">
+        <v>7</v>
+      </c>
+      <c r="I45" s="4">
+        <v>8</v>
+      </c>
+      <c r="J45" s="4">
+        <v>9</v>
+      </c>
+      <c r="K45" s="4">
+        <v>10</v>
+      </c>
+      <c r="L45" s="4">
+        <v>11</v>
+      </c>
+      <c r="M45" s="4">
+        <v>12</v>
+      </c>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+    </row>
+    <row r="46" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4">
+        <v>4</v>
+      </c>
+      <c r="F46" s="4">
+        <v>5</v>
+      </c>
+      <c r="G46" s="4">
+        <v>6</v>
+      </c>
+      <c r="H46" s="4">
+        <v>7</v>
+      </c>
+      <c r="I46" s="4">
+        <v>8</v>
+      </c>
+      <c r="J46" s="4">
+        <v>9</v>
+      </c>
+      <c r="K46" s="4">
+        <v>10</v>
+      </c>
+      <c r="L46" s="4">
+        <v>11</v>
+      </c>
+      <c r="M46" s="4">
+        <v>12</v>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+    </row>
+    <row r="47" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4">
+        <v>3</v>
+      </c>
+      <c r="E47" s="4">
+        <v>4</v>
+      </c>
+      <c r="F47" s="4">
+        <v>5</v>
+      </c>
+      <c r="G47" s="4">
+        <v>6</v>
+      </c>
+      <c r="H47" s="4">
+        <v>7</v>
+      </c>
+      <c r="I47" s="4">
+        <v>8</v>
+      </c>
+      <c r="J47" s="4">
+        <v>9</v>
+      </c>
+      <c r="K47" s="4">
+        <v>10</v>
+      </c>
+      <c r="L47" s="4">
+        <v>11</v>
+      </c>
+      <c r="M47" s="4">
+        <v>12</v>
+      </c>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+    </row>
+    <row r="48" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="7">
+        <v>2</v>
+      </c>
+      <c r="D48" s="7">
+        <v>3</v>
+      </c>
+      <c r="E48" s="7">
+        <v>4</v>
+      </c>
+      <c r="F48" s="7">
+        <v>5</v>
+      </c>
+      <c r="G48" s="7">
+        <v>6</v>
+      </c>
+      <c r="H48" s="7">
+        <v>7</v>
+      </c>
+      <c r="I48" s="7">
+        <v>8</v>
+      </c>
+      <c r="J48" s="7">
+        <v>9</v>
+      </c>
+      <c r="K48" s="7">
+        <v>10</v>
+      </c>
+      <c r="L48" s="7">
+        <v>11</v>
+      </c>
+      <c r="M48" s="7">
+        <v>12</v>
+      </c>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2</v>
+      </c>
+      <c r="D49" s="7">
+        <v>3</v>
+      </c>
+      <c r="E49" s="7">
+        <v>4</v>
+      </c>
+      <c r="F49" s="7">
+        <v>5</v>
+      </c>
+      <c r="G49" s="7">
+        <v>6</v>
+      </c>
+      <c r="H49" s="7">
+        <v>7</v>
+      </c>
+      <c r="I49" s="7">
+        <v>8</v>
+      </c>
+      <c r="J49" s="7">
+        <v>9</v>
+      </c>
+      <c r="K49" s="7">
+        <v>10</v>
+      </c>
+      <c r="L49" s="7">
+        <v>11</v>
+      </c>
+      <c r="M49" s="7">
+        <v>12</v>
+      </c>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+    </row>
+    <row r="50" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="6">
+        <v>1</v>
+      </c>
+      <c r="C50" s="7">
+        <v>2</v>
+      </c>
+      <c r="D50" s="7">
+        <v>3</v>
+      </c>
+      <c r="E50" s="7">
+        <v>4</v>
+      </c>
+      <c r="F50" s="7">
+        <v>5</v>
+      </c>
+      <c r="G50" s="7">
+        <v>6</v>
+      </c>
+      <c r="H50" s="7">
+        <v>7</v>
+      </c>
+      <c r="I50" s="7">
+        <v>8</v>
+      </c>
+      <c r="J50" s="7">
+        <v>9</v>
+      </c>
+      <c r="K50" s="7">
+        <v>10</v>
+      </c>
+      <c r="L50" s="7">
+        <v>11</v>
+      </c>
+      <c r="M50" s="7">
+        <v>12</v>
+      </c>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+    </row>
+    <row r="51" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>3</v>
+      </c>
+      <c r="E51" s="7">
+        <v>4</v>
+      </c>
+      <c r="F51" s="7">
+        <v>5</v>
+      </c>
+      <c r="G51" s="7">
+        <v>6</v>
+      </c>
+      <c r="H51" s="7">
+        <v>7</v>
+      </c>
+      <c r="I51" s="7">
+        <v>8</v>
+      </c>
+      <c r="J51" s="7">
+        <v>9</v>
+      </c>
+      <c r="K51" s="7">
+        <v>10</v>
+      </c>
+      <c r="L51" s="7">
+        <v>11</v>
+      </c>
+      <c r="M51" s="7">
+        <v>12</v>
+      </c>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+    </row>
+    <row r="52" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="7">
+        <v>2</v>
+      </c>
+      <c r="D52" s="7">
+        <v>3</v>
+      </c>
+      <c r="E52" s="7">
+        <v>4</v>
+      </c>
+      <c r="F52" s="7">
+        <v>5</v>
+      </c>
+      <c r="G52" s="7">
+        <v>6</v>
+      </c>
+      <c r="H52" s="7">
+        <v>7</v>
+      </c>
+      <c r="I52" s="7">
+        <v>8</v>
+      </c>
+      <c r="J52" s="7">
+        <v>9</v>
+      </c>
+      <c r="K52" s="7">
+        <v>10</v>
+      </c>
+      <c r="L52" s="7">
+        <v>11</v>
+      </c>
+      <c r="M52" s="7">
+        <v>12</v>
+      </c>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+    </row>
+    <row r="53" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="8">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9">
+        <v>2</v>
+      </c>
+      <c r="D53" s="9">
+        <v>3</v>
+      </c>
+      <c r="E53" s="9">
+        <v>4</v>
+      </c>
+      <c r="F53" s="9">
+        <v>5</v>
+      </c>
+      <c r="G53" s="9">
+        <v>6</v>
+      </c>
+      <c r="H53" s="9">
+        <v>7</v>
+      </c>
+      <c r="I53" s="9">
+        <v>8</v>
+      </c>
+      <c r="J53" s="9">
+        <v>9</v>
+      </c>
+      <c r="K53" s="9">
+        <v>10</v>
+      </c>
+      <c r="L53" s="9">
+        <v>11</v>
+      </c>
+      <c r="M53" s="9">
+        <v>12</v>
+      </c>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+    </row>
+    <row r="54" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="8">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9">
+        <v>2</v>
+      </c>
+      <c r="D54" s="9">
+        <v>3</v>
+      </c>
+      <c r="E54" s="9">
+        <v>4</v>
+      </c>
+      <c r="F54" s="9">
+        <v>5</v>
+      </c>
+      <c r="G54" s="9">
+        <v>6</v>
+      </c>
+      <c r="H54" s="9">
+        <v>7</v>
+      </c>
+      <c r="I54" s="9">
+        <v>8</v>
+      </c>
+      <c r="J54" s="9">
+        <v>9</v>
+      </c>
+      <c r="K54" s="9">
+        <v>10</v>
+      </c>
+      <c r="L54" s="9">
+        <v>11</v>
+      </c>
+      <c r="M54" s="9">
+        <v>12</v>
+      </c>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+    </row>
+    <row r="55" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="8">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9">
+        <v>2</v>
+      </c>
+      <c r="D55" s="9">
+        <v>3</v>
+      </c>
+      <c r="E55" s="9">
+        <v>4</v>
+      </c>
+      <c r="F55" s="9">
+        <v>5</v>
+      </c>
+      <c r="G55" s="9">
+        <v>6</v>
+      </c>
+      <c r="H55" s="9">
+        <v>7</v>
+      </c>
+      <c r="I55" s="9">
+        <v>8</v>
+      </c>
+      <c r="J55" s="9">
+        <v>9</v>
+      </c>
+      <c r="K55" s="9">
+        <v>10</v>
+      </c>
+      <c r="L55" s="9">
+        <v>11</v>
+      </c>
+      <c r="M55" s="9">
+        <v>12</v>
+      </c>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+    </row>
+    <row r="56" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="8">
+        <v>1</v>
+      </c>
+      <c r="C56" s="9">
+        <v>2</v>
+      </c>
+      <c r="D56" s="9">
+        <v>3</v>
+      </c>
+      <c r="E56" s="9">
+        <v>4</v>
+      </c>
+      <c r="F56" s="9">
+        <v>5</v>
+      </c>
+      <c r="G56" s="9">
+        <v>6</v>
+      </c>
+      <c r="H56" s="9">
+        <v>7</v>
+      </c>
+      <c r="I56" s="9">
+        <v>8</v>
+      </c>
+      <c r="J56" s="9">
+        <v>9</v>
+      </c>
+      <c r="K56" s="9">
+        <v>10</v>
+      </c>
+      <c r="L56" s="9">
+        <v>11</v>
+      </c>
+      <c r="M56" s="9">
+        <v>12</v>
+      </c>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+    </row>
+    <row r="57" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="8">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9">
+        <v>2</v>
+      </c>
+      <c r="D57" s="9">
+        <v>3</v>
+      </c>
+      <c r="E57" s="9">
+        <v>4</v>
+      </c>
+      <c r="F57" s="9">
+        <v>5</v>
+      </c>
+      <c r="G57" s="9">
+        <v>6</v>
+      </c>
+      <c r="H57" s="9">
+        <v>7</v>
+      </c>
+      <c r="I57" s="9">
+        <v>8</v>
+      </c>
+      <c r="J57" s="9">
+        <v>9</v>
+      </c>
+      <c r="K57" s="9">
+        <v>10</v>
+      </c>
+      <c r="L57" s="9">
+        <v>11</v>
+      </c>
+      <c r="M57" s="9">
+        <v>12</v>
+      </c>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <f xml:space="preserve"> SUM(B43,B42,A43,B44,C43)</f>
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ref="C63:M63" si="3" xml:space="preserve"> SUM(C43,C42,B43,C44,D43)</f>
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <f t="shared" ref="B64:M64" si="4" xml:space="preserve"> SUM(B44,B43,A44,B45,C44)</f>
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <f t="shared" ref="B65:M65" si="5" xml:space="preserve"> SUM(B45,B44,A45,B46,C45)</f>
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <f t="shared" ref="B66:M66" si="6" xml:space="preserve"> SUM(B46,B45,A46,B47,C46)</f>
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="6"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f t="shared" ref="B67:M67" si="7" xml:space="preserve"> SUM(B47,B46,A47,B48,C47)</f>
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <f t="shared" ref="B68:M68" si="8" xml:space="preserve"> SUM(B48,B47,A48,B49,C48)</f>
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <f t="shared" ref="B69:M69" si="9" xml:space="preserve"> SUM(B49,B48,A49,B50,C49)</f>
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="9"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <f t="shared" ref="B70:M70" si="10" xml:space="preserve"> SUM(B50,B49,A50,B51,C50)</f>
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="10"/>
+        <v>55</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="10"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <f t="shared" ref="B71:M71" si="11" xml:space="preserve"> SUM(B51,B50,A51,B52,C51)</f>
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="11"/>
+        <v>35</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="11"/>
+        <v>55</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="11"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <f t="shared" ref="B72:M72" si="12" xml:space="preserve"> SUM(B52,B51,A52,B53,C52)</f>
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="12"/>
+        <v>35</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="12"/>
+        <v>45</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="12"/>
+        <v>50</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="12"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <f t="shared" ref="B73:M73" si="13" xml:space="preserve"> SUM(B53,B52,A53,B54,C53)</f>
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="13"/>
+        <v>25</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="13"/>
+        <v>35</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="13"/>
+        <v>40</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="13"/>
+        <v>55</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="13"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <f t="shared" ref="B74:M74" si="14" xml:space="preserve"> SUM(B54,B53,A54,B55,C54)</f>
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="14"/>
+        <v>25</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="14"/>
+        <v>30</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="14"/>
+        <v>35</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="14"/>
+        <v>40</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="14"/>
+        <v>45</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="14"/>
+        <v>50</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="14"/>
+        <v>55</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="14"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <f t="shared" ref="B75:M75" si="15" xml:space="preserve"> SUM(B55,B54,A55,B56,C55)</f>
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="15"/>
+        <v>35</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="15"/>
+        <v>45</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="15"/>
+        <v>50</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="15"/>
+        <v>55</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="15"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <f t="shared" ref="B76:M76" si="16" xml:space="preserve"> SUM(B56,B55,A56,B57,C56)</f>
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="16"/>
+        <v>40</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="16"/>
+        <v>45</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="16"/>
+        <v>50</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="16"/>
+        <v>55</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="16"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <f t="shared" ref="B77:M77" si="17" xml:space="preserve"> SUM(B57,B56,A57,B58,C57)</f>
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="17"/>
+        <v>28</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="17"/>
+        <v>32</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="17"/>
+        <v>36</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="17"/>
+        <v>44</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="17"/>
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>